<commit_message>
Include comment in answer exports (#454)
</commit_message>
<xml_diff>
--- a/tests/export/answers.xlsx
+++ b/tests/export/answers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Participant name</t>
   </si>
@@ -31,6 +31,9 @@
     <t>2019-09-12T13:30</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>Albert Einstein</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t>available</t>
+  </si>
+  <si>
+    <t>Available comment</t>
   </si>
 </sst>
 </file>
@@ -387,13 +393,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,29 +415,38 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TextIOWrapper instead of StringIO buffer
</commit_message>
<xml_diff>
--- a/tests/export/answers.xlsx
+++ b/tests/export/answers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Participant name</t>
   </si>
@@ -46,13 +46,16 @@
     <t>ifneedbe</t>
   </si>
   <si>
+    <t>Hello world</t>
+  </si>
+  <si>
     <t>Tony Stark</t>
   </si>
   <si>
     <t>available</t>
   </si>
   <si>
-    <t>Available, comment</t>
+    <t>Hello, world</t>
   </si>
 </sst>
 </file>
@@ -435,18 +438,18 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use CSV writer for answer exports (#456)
</commit_message>
<xml_diff>
--- a/tests/export/answers.xlsx
+++ b/tests/export/answers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Participant name</t>
   </si>
@@ -46,13 +46,16 @@
     <t>ifneedbe</t>
   </si>
   <si>
+    <t>Hello world</t>
+  </si>
+  <si>
     <t>Tony Stark</t>
   </si>
   <si>
     <t>available</t>
   </si>
   <si>
-    <t>Available comment</t>
+    <t>Hello, world</t>
   </si>
 </sst>
 </file>
@@ -435,18 +438,18 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>